<commit_message>
Added `...` back to top-level functions (Which work); they only seem to break if passed _lower_.
</commit_message>
<xml_diff>
--- a/inst/examples/xlsx.xlsx
+++ b/inst/examples/xlsx.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>testheader1</t>
   </si>
@@ -109,12 +110,18 @@
   </si>
   <si>
     <t>testdata44</t>
+  </si>
+  <si>
+    <t>sheet_test</t>
+  </si>
+  <si>
+    <t>this is just a test for passing Excel sheets as a readit argument</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,7 +432,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -539,4 +546,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>